<commit_message>
js FP & OO concepts
</commit_message>
<xml_diff>
--- a/XT_FULLSTACK_TRAINING_16_Weeks - updated_new.xlsx
+++ b/XT_FULLSTACK_TRAINING_16_Weeks - updated_new.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Trainer Plan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -2166,7 +2167,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2516,6 +2517,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3014,7 +3017,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3044,29 +3047,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12" ht="19" customHeight="1">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="129" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="131" t="s">
+      <c r="C3" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="131"/>
-      <c r="E3" s="131"/>
-      <c r="F3" s="131"/>
-      <c r="G3" s="131" t="s">
+      <c r="D3" s="133"/>
+      <c r="E3" s="133"/>
+      <c r="F3" s="133"/>
+      <c r="G3" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="131"/>
-      <c r="I3" s="131"/>
-      <c r="J3" s="131"/>
-      <c r="K3" s="131"/>
-      <c r="L3" s="131"/>
+      <c r="H3" s="133"/>
+      <c r="I3" s="133"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="133"/>
+      <c r="L3" s="133"/>
     </row>
     <row r="4" spans="1:12" s="7" customFormat="1" ht="16" thickBot="1">
-      <c r="A4" s="127"/>
+      <c r="A4" s="129"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -3102,7 +3105,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="31" thickBot="1">
-      <c r="A5" s="127"/>
+      <c r="A5" s="129"/>
       <c r="B5" s="78" t="s">
         <v>15</v>
       </c>
@@ -3138,7 +3141,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="19" customHeight="1" thickBot="1">
-      <c r="A6" s="127"/>
+      <c r="A6" s="129"/>
       <c r="B6" s="79" t="s">
         <v>24</v>
       </c>
@@ -3174,7 +3177,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="31" thickBot="1">
-      <c r="A7" s="127"/>
+      <c r="A7" s="129"/>
       <c r="B7" s="79" t="s">
         <v>34</v>
       </c>
@@ -3210,7 +3213,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="19" customHeight="1" thickBot="1">
-      <c r="A8" s="127"/>
+      <c r="A8" s="129"/>
       <c r="B8" s="24"/>
       <c r="C8" s="57" t="s">
         <v>45</v>
@@ -3244,7 +3247,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="30">
-      <c r="A9" s="127"/>
+      <c r="A9" s="129"/>
       <c r="B9" s="24"/>
       <c r="C9" s="57" t="s">
         <v>55</v>
@@ -3278,7 +3281,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="30">
-      <c r="A10" s="127"/>
+      <c r="A10" s="129"/>
       <c r="B10" s="24"/>
       <c r="C10" s="57" t="s">
         <v>65</v>
@@ -3312,7 +3315,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="19" customHeight="1">
-      <c r="A11" s="127"/>
+      <c r="A11" s="129"/>
       <c r="B11" s="8"/>
       <c r="C11" s="25" t="s">
         <v>75</v>
@@ -3344,7 +3347,7 @@
       <c r="L11" s="26"/>
     </row>
     <row r="12" spans="1:12" ht="40" customHeight="1">
-      <c r="A12" s="127"/>
+      <c r="A12" s="129"/>
       <c r="B12" s="8"/>
       <c r="C12" s="40" t="s">
         <v>84</v>
@@ -3374,7 +3377,7 @@
       <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:12" ht="30">
-      <c r="A13" s="127"/>
+      <c r="A13" s="129"/>
       <c r="B13" s="8"/>
       <c r="C13" s="25" t="s">
         <v>91</v>
@@ -3400,7 +3403,7 @@
       <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:12" ht="19" customHeight="1">
-      <c r="A14" s="127"/>
+      <c r="A14" s="129"/>
       <c r="B14" s="8"/>
       <c r="C14" s="81" t="s">
         <v>97</v>
@@ -3424,7 +3427,7 @@
       <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:12" ht="19" customHeight="1">
-      <c r="A15" s="127"/>
+      <c r="A15" s="129"/>
       <c r="B15" s="8"/>
       <c r="C15" s="25" t="s">
         <v>101</v>
@@ -3446,7 +3449,7 @@
       <c r="L15" s="26"/>
     </row>
     <row r="16" spans="1:12" ht="19" customHeight="1">
-      <c r="A16" s="127"/>
+      <c r="A16" s="129"/>
       <c r="B16" s="8"/>
       <c r="C16" s="40" t="s">
         <v>294</v>
@@ -3468,7 +3471,7 @@
       <c r="L16" s="26"/>
     </row>
     <row r="17" spans="1:12" ht="19" customHeight="1">
-      <c r="A17" s="127"/>
+      <c r="A17" s="129"/>
       <c r="B17" s="8"/>
       <c r="C17" s="25" t="s">
         <v>108</v>
@@ -3490,7 +3493,7 @@
       <c r="L17" s="26"/>
     </row>
     <row r="18" spans="1:12" ht="19" customHeight="1">
-      <c r="A18" s="127"/>
+      <c r="A18" s="129"/>
       <c r="B18" s="8"/>
       <c r="C18" s="25" t="s">
         <v>111</v>
@@ -3510,7 +3513,7 @@
       <c r="L18" s="26"/>
     </row>
     <row r="19" spans="1:12" ht="19" customHeight="1">
-      <c r="A19" s="127"/>
+      <c r="A19" s="129"/>
       <c r="B19" s="8"/>
       <c r="C19" s="40" t="s">
         <v>114</v>
@@ -3530,7 +3533,7 @@
       <c r="L19" s="26"/>
     </row>
     <row r="20" spans="1:12" ht="19" customHeight="1">
-      <c r="A20" s="127"/>
+      <c r="A20" s="129"/>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
       <c r="D20" s="27"/>
@@ -3548,7 +3551,7 @@
       <c r="L20" s="26"/>
     </row>
     <row r="21" spans="1:12" ht="19" customHeight="1">
-      <c r="A21" s="127"/>
+      <c r="A21" s="129"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="27"/>
@@ -3566,7 +3569,7 @@
       <c r="L21" s="26"/>
     </row>
     <row r="22" spans="1:12" ht="19" customHeight="1">
-      <c r="A22" s="127"/>
+      <c r="A22" s="129"/>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
       <c r="D22" s="27"/>
@@ -3584,7 +3587,7 @@
       <c r="L22" s="26"/>
     </row>
     <row r="23" spans="1:12" ht="19" customHeight="1">
-      <c r="A23" s="127"/>
+      <c r="A23" s="129"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="27"/>
@@ -3602,7 +3605,7 @@
       <c r="L23" s="26"/>
     </row>
     <row r="24" spans="1:12" ht="19" customHeight="1">
-      <c r="A24" s="127"/>
+      <c r="A24" s="129"/>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="27"/>
@@ -3620,7 +3623,7 @@
       <c r="L24" s="26"/>
     </row>
     <row r="25" spans="1:12" ht="30">
-      <c r="A25" s="127"/>
+      <c r="A25" s="129"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="27"/>
@@ -3638,7 +3641,7 @@
       <c r="L25" s="26"/>
     </row>
     <row r="26" spans="1:12" ht="19" customHeight="1">
-      <c r="A26" s="127"/>
+      <c r="A26" s="129"/>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
       <c r="D26" s="27"/>
@@ -3656,7 +3659,7 @@
       <c r="L26" s="26"/>
     </row>
     <row r="27" spans="1:12" ht="19" customHeight="1">
-      <c r="A27" s="127"/>
+      <c r="A27" s="129"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="27"/>
@@ -3674,7 +3677,7 @@
       <c r="L27" s="26"/>
     </row>
     <row r="28" spans="1:12" ht="19" customHeight="1">
-      <c r="A28" s="127"/>
+      <c r="A28" s="129"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="27"/>
@@ -3692,7 +3695,7 @@
       <c r="L28" s="26"/>
     </row>
     <row r="29" spans="1:12" ht="19" customHeight="1">
-      <c r="A29" s="127"/>
+      <c r="A29" s="129"/>
       <c r="B29" s="8"/>
       <c r="C29" s="9"/>
       <c r="D29" s="27"/>
@@ -3708,7 +3711,7 @@
       <c r="L29" s="26"/>
     </row>
     <row r="30" spans="1:12" ht="19" customHeight="1">
-      <c r="A30" s="127"/>
+      <c r="A30" s="129"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
       <c r="D30" s="30"/>
@@ -3738,27 +3741,27 @@
       <c r="L32" s="12"/>
     </row>
     <row r="34" spans="1:12" ht="19" customHeight="1">
-      <c r="A34" s="127" t="s">
+      <c r="A34" s="129" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="132" t="s">
+      <c r="B34" s="134" t="s">
         <v>138</v>
       </c>
-      <c r="C34" s="132"/>
-      <c r="D34" s="132"/>
-      <c r="E34" s="132"/>
-      <c r="F34" s="132"/>
-      <c r="G34" s="132"/>
-      <c r="H34" s="132"/>
-      <c r="I34" s="131" t="s">
+      <c r="C34" s="134"/>
+      <c r="D34" s="134"/>
+      <c r="E34" s="134"/>
+      <c r="F34" s="134"/>
+      <c r="G34" s="134"/>
+      <c r="H34" s="134"/>
+      <c r="I34" s="133" t="s">
         <v>139</v>
       </c>
-      <c r="J34" s="131"/>
-      <c r="K34" s="131"/>
-      <c r="L34" s="131"/>
+      <c r="J34" s="133"/>
+      <c r="K34" s="133"/>
+      <c r="L34" s="133"/>
     </row>
     <row r="35" spans="1:12" ht="19" customHeight="1">
-      <c r="A35" s="127"/>
+      <c r="A35" s="129"/>
       <c r="B35" s="13" t="s">
         <v>140</v>
       </c>
@@ -3792,7 +3795,7 @@
       <c r="L35" s="18"/>
     </row>
     <row r="36" spans="1:12" ht="45">
-      <c r="A36" s="127"/>
+      <c r="A36" s="129"/>
       <c r="B36" s="50" t="s">
         <v>150</v>
       </c>
@@ -3826,7 +3829,7 @@
       <c r="L36" s="34"/>
     </row>
     <row r="37" spans="1:12" ht="45">
-      <c r="A37" s="127"/>
+      <c r="A37" s="129"/>
       <c r="B37" s="40" t="s">
         <v>157</v>
       </c>
@@ -3860,7 +3863,7 @@
       <c r="L37" s="26"/>
     </row>
     <row r="38" spans="1:12" ht="30">
-      <c r="A38" s="127"/>
+      <c r="A38" s="129"/>
       <c r="B38" s="40" t="s">
         <v>167</v>
       </c>
@@ -3894,7 +3897,7 @@
       <c r="L38" s="26"/>
     </row>
     <row r="39" spans="1:12" ht="30">
-      <c r="A39" s="127"/>
+      <c r="A39" s="129"/>
       <c r="B39" s="40" t="s">
         <v>176</v>
       </c>
@@ -3926,7 +3929,7 @@
       <c r="L39" s="26"/>
     </row>
     <row r="40" spans="1:12" ht="30">
-      <c r="A40" s="127"/>
+      <c r="A40" s="129"/>
       <c r="B40" s="40" t="s">
         <v>185</v>
       </c>
@@ -3958,7 +3961,7 @@
       <c r="L40" s="26"/>
     </row>
     <row r="41" spans="1:12" ht="30">
-      <c r="A41" s="127"/>
+      <c r="A41" s="129"/>
       <c r="B41" s="40" t="s">
         <v>193</v>
       </c>
@@ -3988,7 +3991,7 @@
       <c r="L41" s="26"/>
     </row>
     <row r="42" spans="1:12" ht="19" customHeight="1">
-      <c r="A42" s="127"/>
+      <c r="A42" s="129"/>
       <c r="B42" s="40" t="s">
         <v>200</v>
       </c>
@@ -4016,7 +4019,7 @@
       <c r="L42" s="26"/>
     </row>
     <row r="43" spans="1:12" ht="30">
-      <c r="A43" s="127"/>
+      <c r="A43" s="129"/>
       <c r="B43" s="40" t="s">
         <v>207</v>
       </c>
@@ -4042,7 +4045,7 @@
       <c r="L43" s="26"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="127"/>
+      <c r="A44" s="129"/>
       <c r="B44" s="40" t="s">
         <v>213</v>
       </c>
@@ -4068,7 +4071,7 @@
       <c r="L44" s="26"/>
     </row>
     <row r="45" spans="1:12" ht="30">
-      <c r="A45" s="127"/>
+      <c r="A45" s="129"/>
       <c r="B45" s="40" t="s">
         <v>219</v>
       </c>
@@ -4092,7 +4095,7 @@
       <c r="L45" s="26"/>
     </row>
     <row r="46" spans="1:12" ht="19" customHeight="1">
-      <c r="A46" s="127"/>
+      <c r="A46" s="129"/>
       <c r="B46" s="40" t="s">
         <v>223</v>
       </c>
@@ -4114,7 +4117,7 @@
       <c r="L46" s="26"/>
     </row>
     <row r="47" spans="1:12" ht="19" customHeight="1">
-      <c r="A47" s="127"/>
+      <c r="A47" s="129"/>
       <c r="B47" s="40" t="s">
         <v>227</v>
       </c>
@@ -4136,7 +4139,7 @@
       <c r="L47" s="26"/>
     </row>
     <row r="48" spans="1:12" ht="19" customHeight="1">
-      <c r="A48" s="127"/>
+      <c r="A48" s="129"/>
       <c r="B48" s="40" t="s">
         <v>230</v>
       </c>
@@ -4156,7 +4159,7 @@
       <c r="L48" s="26"/>
     </row>
     <row r="49" spans="1:12" ht="19" customHeight="1">
-      <c r="A49" s="127"/>
+      <c r="A49" s="129"/>
       <c r="B49" s="40" t="s">
         <v>232</v>
       </c>
@@ -4176,7 +4179,7 @@
       <c r="L49" s="26"/>
     </row>
     <row r="50" spans="1:12" ht="19" customHeight="1">
-      <c r="A50" s="127"/>
+      <c r="A50" s="129"/>
       <c r="B50" s="40" t="s">
         <v>235</v>
       </c>
@@ -4196,7 +4199,7 @@
       <c r="L50" s="26"/>
     </row>
     <row r="51" spans="1:12" ht="19" customHeight="1">
-      <c r="A51" s="127"/>
+      <c r="A51" s="129"/>
       <c r="B51" s="40" t="s">
         <v>300</v>
       </c>
@@ -4216,7 +4219,7 @@
       <c r="L51" s="26"/>
     </row>
     <row r="52" spans="1:12" ht="19" customHeight="1">
-      <c r="A52" s="127"/>
+      <c r="A52" s="129"/>
       <c r="B52" s="51" t="s">
         <v>240</v>
       </c>
@@ -4232,7 +4235,7 @@
       <c r="L52" s="37"/>
     </row>
     <row r="53" spans="1:12" ht="19" customHeight="1">
-      <c r="A53" s="127"/>
+      <c r="A53" s="129"/>
       <c r="B53" s="52" t="s">
         <v>241</v>
       </c>
@@ -4264,25 +4267,25 @@
       <c r="L55" s="19"/>
     </row>
     <row r="57" spans="1:12" ht="19" customHeight="1">
-      <c r="A57" s="127" t="s">
+      <c r="A57" s="129" t="s">
         <v>242</v>
       </c>
-      <c r="B57" s="128" t="s">
+      <c r="B57" s="130" t="s">
         <v>243</v>
       </c>
-      <c r="C57" s="128"/>
-      <c r="D57" s="128"/>
-      <c r="E57" s="128"/>
-      <c r="F57" s="128"/>
-      <c r="G57" s="128"/>
-      <c r="H57" s="128"/>
-      <c r="I57" s="128"/>
-      <c r="J57" s="128"/>
-      <c r="K57" s="128"/>
-      <c r="L57" s="128"/>
+      <c r="C57" s="130"/>
+      <c r="D57" s="130"/>
+      <c r="E57" s="130"/>
+      <c r="F57" s="130"/>
+      <c r="G57" s="130"/>
+      <c r="H57" s="130"/>
+      <c r="I57" s="130"/>
+      <c r="J57" s="130"/>
+      <c r="K57" s="130"/>
+      <c r="L57" s="130"/>
     </row>
     <row r="58" spans="1:12" ht="19" customHeight="1">
-      <c r="A58" s="127"/>
+      <c r="A58" s="129"/>
       <c r="B58" s="20" t="s">
         <v>244</v>
       </c>
@@ -4318,11 +4321,11 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="26.25" customHeight="1">
-      <c r="A59" s="127"/>
-      <c r="B59" s="129" t="s">
+      <c r="A59" s="129"/>
+      <c r="B59" s="131" t="s">
         <v>255</v>
       </c>
-      <c r="C59" s="130" t="s">
+      <c r="C59" s="132" t="s">
         <v>301</v>
       </c>
       <c r="D59" s="49" t="s">
@@ -4354,9 +4357,9 @@
       </c>
     </row>
     <row r="60" spans="1:12" ht="19" customHeight="1">
-      <c r="A60" s="127"/>
-      <c r="B60" s="129"/>
-      <c r="C60" s="130"/>
+      <c r="A60" s="129"/>
+      <c r="B60" s="131"/>
+      <c r="C60" s="132"/>
       <c r="D60" s="43" t="s">
         <v>265</v>
       </c>
@@ -4380,7 +4383,7 @@
       </c>
     </row>
     <row r="61" spans="1:12">
-      <c r="A61" s="127"/>
+      <c r="A61" s="129"/>
       <c r="B61" s="28"/>
       <c r="C61" s="43" t="s">
         <v>271</v>
@@ -4408,7 +4411,7 @@
       </c>
     </row>
     <row r="62" spans="1:12" ht="19" customHeight="1">
-      <c r="A62" s="127"/>
+      <c r="A62" s="129"/>
       <c r="B62" s="28"/>
       <c r="C62" s="43" t="s">
         <v>278</v>
@@ -4434,7 +4437,7 @@
       </c>
     </row>
     <row r="63" spans="1:12" ht="19" customHeight="1">
-      <c r="A63" s="127"/>
+      <c r="A63" s="129"/>
       <c r="B63" s="28"/>
       <c r="C63" s="43" t="s">
         <v>284</v>
@@ -4456,7 +4459,7 @@
       <c r="L63" s="26"/>
     </row>
     <row r="64" spans="1:12" ht="19" customHeight="1">
-      <c r="A64" s="127"/>
+      <c r="A64" s="129"/>
       <c r="B64" s="28"/>
       <c r="C64" s="27"/>
       <c r="D64" s="27"/>
@@ -4474,7 +4477,7 @@
       <c r="L64" s="26"/>
     </row>
     <row r="65" spans="1:12" ht="19" customHeight="1">
-      <c r="A65" s="127"/>
+      <c r="A65" s="129"/>
       <c r="B65" s="28"/>
       <c r="C65" s="27"/>
       <c r="D65" s="27"/>
@@ -4490,7 +4493,7 @@
       <c r="L65" s="26"/>
     </row>
     <row r="66" spans="1:12" ht="19" customHeight="1">
-      <c r="A66" s="127"/>
+      <c r="A66" s="129"/>
       <c r="B66" s="28"/>
       <c r="C66" s="27"/>
       <c r="D66" s="27"/>
@@ -4506,7 +4509,7 @@
       <c r="L66" s="26"/>
     </row>
     <row r="67" spans="1:12" ht="30">
-      <c r="A67" s="127"/>
+      <c r="A67" s="129"/>
       <c r="B67" s="32"/>
       <c r="C67" s="30"/>
       <c r="D67" s="30"/>
@@ -4550,7 +4553,7 @@
   <dimension ref="A4:H179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C170" sqref="C170:E172"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
@@ -4577,14 +4580,14 @@
     </row>
     <row r="5" spans="1:5" ht="23">
       <c r="A5" s="82"/>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="138" t="s">
         <v>437</v>
       </c>
-      <c r="C5" s="137"/>
-      <c r="D5" s="138" t="s">
+      <c r="C5" s="139"/>
+      <c r="D5" s="140" t="s">
         <v>438</v>
       </c>
-      <c r="E5" s="139"/>
+      <c r="E5" s="141"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="82"/>
@@ -4939,14 +4942,14 @@
       </c>
     </row>
     <row r="49" spans="2:5" ht="23">
-      <c r="B49" s="140" t="s">
+      <c r="B49" s="142" t="s">
         <v>439</v>
       </c>
-      <c r="C49" s="141"/>
-      <c r="D49" s="138" t="s">
+      <c r="C49" s="143"/>
+      <c r="D49" s="127" t="s">
         <v>441</v>
       </c>
-      <c r="E49" s="139"/>
+      <c r="E49" s="128"/>
     </row>
     <row r="50" spans="2:5" ht="17" customHeight="1"/>
     <row r="51" spans="2:5">
@@ -5303,11 +5306,11 @@
       <c r="B97" s="116" t="s">
         <v>441</v>
       </c>
-      <c r="C97" s="138" t="s">
+      <c r="C97" s="140" t="s">
         <v>440</v>
       </c>
-      <c r="D97" s="142"/>
-      <c r="E97" s="139"/>
+      <c r="D97" s="144"/>
+      <c r="E97" s="141"/>
     </row>
     <row r="100" spans="2:5">
       <c r="B100" s="85" t="s">
@@ -5598,11 +5601,11 @@
       <c r="B140" s="116" t="s">
         <v>442</v>
       </c>
-      <c r="C140" s="133" t="s">
+      <c r="C140" s="135" t="s">
         <v>443</v>
       </c>
-      <c r="D140" s="134"/>
-      <c r="E140" s="135"/>
+      <c r="D140" s="136"/>
+      <c r="E140" s="137"/>
     </row>
     <row r="143" spans="2:5">
       <c r="B143" s="85" t="s">
@@ -5896,9 +5899,8 @@
       <c r="B179" s="111"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="C140:E140"/>
-    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="B49:C49"/>

</xml_diff>